<commit_message>
generate neonic conc. profiles for pollen and nectar from field data
</commit_message>
<xml_diff>
--- a/data/raw/field_neonic_exposure.xlsx
+++ b/data/raw/field_neonic_exposure.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="raw neonic pollen" sheetId="1" r:id="rId1"/>
+    <sheet name="raw neonic clo equivalents" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -66,21 +66,12 @@
     <t>FSR</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>HR</t>
   </si>
   <si>
     <t>IB</t>
   </si>
   <si>
-    <t>MC</t>
-  </si>
-  <si>
-    <t>MM</t>
-  </si>
-  <si>
     <t>SC</t>
   </si>
   <si>
@@ -90,7 +81,79 @@
     <t>WB</t>
   </si>
   <si>
-    <t>Note: FSR 5/2 was a very high outlier. Should use a neighboring value?</t>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>BG - clo</t>
+  </si>
+  <si>
+    <t>DS - thi</t>
+  </si>
+  <si>
+    <t>DS - clo</t>
+  </si>
+  <si>
+    <t>FSR - thi</t>
+  </si>
+  <si>
+    <t>FSR - clo</t>
+  </si>
+  <si>
+    <t>HR - thi</t>
+  </si>
+  <si>
+    <t>HR - clo</t>
+  </si>
+  <si>
+    <t>IB - thi</t>
+  </si>
+  <si>
+    <t>IB - clo</t>
+  </si>
+  <si>
+    <t>SC - thi</t>
+  </si>
+  <si>
+    <t>SC - clo</t>
+  </si>
+  <si>
+    <t>TV - thi</t>
+  </si>
+  <si>
+    <t>BG - thi</t>
+  </si>
+  <si>
+    <t>TV - clo</t>
+  </si>
+  <si>
+    <t>WB - thi</t>
+  </si>
+  <si>
+    <t>WB - clo</t>
+  </si>
+  <si>
+    <t>MB - thi</t>
+  </si>
+  <si>
+    <t>MB - clo</t>
+  </si>
+  <si>
+    <t>MO - thi</t>
+  </si>
+  <si>
+    <t>MO - clo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thi to Clo conversion factor: </t>
+  </si>
+  <si>
+    <t>In clothianidin equivalents:</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -107,7 +170,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -451,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,354 +524,1097 @@
     <col min="1" max="1" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="K1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>4.0250000000000004</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="C2">
-        <v>11.436999999999999</v>
+        <v>3.823</v>
       </c>
       <c r="D2">
-        <v>3.0339999999999998</v>
+        <v>3.448</v>
       </c>
       <c r="E2">
-        <v>1.0209999999999999</v>
+        <v>7.9889999999999999</v>
       </c>
       <c r="F2">
-        <v>6.3879999999999999</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="G2">
-        <v>0.82000000000000006</v>
+        <v>2.8319999999999999</v>
       </c>
       <c r="H2">
-        <v>5.1509999999999998</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="I2">
-        <v>0.82000000000000006</v>
+        <v>0.81899999999999995</v>
       </c>
       <c r="J2">
-        <v>4.5670000000000002</v>
+        <v>2.641</v>
       </c>
       <c r="K2">
-        <v>13.867000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3.7469999999999999</v>
+      </c>
+      <c r="L2">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="M2">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="N2">
+        <v>1.254</v>
+      </c>
+      <c r="O2">
+        <v>3.8969999999999998</v>
+      </c>
+      <c r="P2">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="Q2">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="R2">
+        <v>2.806</v>
+      </c>
+      <c r="S2">
+        <v>1.7609999999999999</v>
+      </c>
+      <c r="T2">
+        <v>7.5170000000000003</v>
+      </c>
+      <c r="U2">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>7.2940000000000005</v>
+        <v>3.0470000000000002</v>
       </c>
       <c r="C3">
-        <v>10.382000000000001</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>4.2469999999999999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5.0910000000000002</v>
       </c>
       <c r="E3">
-        <v>12.916</v>
-      </c>
-      <c r="F3">
-        <v>6.633</v>
-      </c>
-      <c r="G3">
-        <v>21.731000000000002</v>
+        <v>5.2910000000000004</v>
       </c>
       <c r="H3">
-        <v>11.675000000000001</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="I3">
-        <v>50.478000000000002</v>
+        <v>12.714</v>
       </c>
       <c r="J3">
-        <v>17.013999999999999</v>
+        <v>1.5469999999999999</v>
       </c>
       <c r="K3">
-        <v>12.468</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>5.0860000000000003</v>
+      </c>
+      <c r="L3">
+        <v>3.673</v>
+      </c>
+      <c r="M3">
+        <v>18.058</v>
+      </c>
+      <c r="N3">
+        <v>2.7160000000000002</v>
+      </c>
+      <c r="O3">
+        <v>8.9589999999999996</v>
+      </c>
+      <c r="P3">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="Q3">
+        <v>50.276000000000003</v>
+      </c>
+      <c r="R3">
+        <v>1.6719999999999999</v>
+      </c>
+      <c r="S3">
+        <v>15.342000000000001</v>
+      </c>
+      <c r="T3">
+        <v>3.5960000000000001</v>
+      </c>
+      <c r="U3">
+        <v>8.8719999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>35.853000000000002</v>
+        <v>24.048999999999999</v>
       </c>
       <c r="C4">
-        <v>10.058</v>
+        <v>11.804</v>
       </c>
       <c r="D4">
-        <v>65.986000000000004</v>
+        <v>2.968</v>
       </c>
       <c r="E4">
-        <v>21.032</v>
+        <v>7.09</v>
       </c>
       <c r="F4">
-        <v>14.14</v>
+        <v>19.050999999999998</v>
       </c>
       <c r="G4">
-        <v>12.884</v>
+        <v>46.935000000000002</v>
       </c>
       <c r="H4">
-        <v>25.385999999999999</v>
+        <v>3.28</v>
       </c>
       <c r="I4">
-        <v>15.552</v>
+        <v>17.751999999999999</v>
       </c>
       <c r="J4">
-        <v>54.636000000000003</v>
+        <v>3.2130000000000001</v>
       </c>
       <c r="K4">
-        <v>29.706000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10.927</v>
+      </c>
+      <c r="L4">
+        <v>3.0289999999999999</v>
+      </c>
+      <c r="M4">
+        <v>9.8550000000000004</v>
+      </c>
+      <c r="N4">
+        <v>1.8720000000000001</v>
+      </c>
+      <c r="O4">
+        <v>23.513999999999999</v>
+      </c>
+      <c r="P4">
+        <v>5.226</v>
+      </c>
+      <c r="Q4">
+        <v>10.326000000000001</v>
+      </c>
+      <c r="R4">
+        <v>16.692</v>
+      </c>
+      <c r="S4">
+        <v>37.944000000000003</v>
+      </c>
+      <c r="T4">
+        <v>10.101000000000001</v>
+      </c>
+      <c r="U4">
+        <v>19.605</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>21.797000000000001</v>
+        <v>8.1690000000000005</v>
       </c>
       <c r="C5">
-        <v>10.411</v>
+        <v>13.628</v>
       </c>
       <c r="D5">
-        <v>3.61</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="E5">
-        <v>50.202999999999996</v>
+        <v>10.026</v>
       </c>
       <c r="F5">
-        <v>14.721</v>
+        <v>1.387</v>
       </c>
       <c r="G5">
-        <v>9.1280000000000001</v>
+        <v>2.2229999999999999</v>
       </c>
       <c r="H5">
-        <v>12.632999999999999</v>
+        <v>15.391</v>
       </c>
       <c r="I5">
-        <v>6.28</v>
+        <v>34.811999999999998</v>
       </c>
       <c r="J5">
-        <v>10.298</v>
+        <v>6.7370000000000001</v>
       </c>
       <c r="K5">
-        <v>25.872999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>7.984</v>
+      </c>
+      <c r="L5">
+        <v>5.2530000000000001</v>
+      </c>
+      <c r="M5">
+        <v>3.875</v>
+      </c>
+      <c r="N5">
+        <v>3.226</v>
+      </c>
+      <c r="O5">
+        <v>9.407</v>
+      </c>
+      <c r="P5">
+        <v>2.1909999999999998</v>
+      </c>
+      <c r="Q5">
+        <v>4.0890000000000004</v>
+      </c>
+      <c r="R5">
+        <v>2.7440000000000002</v>
+      </c>
+      <c r="S5">
+        <v>7.5540000000000003</v>
+      </c>
+      <c r="T5">
+        <v>20.462</v>
+      </c>
+      <c r="U5">
+        <v>5.4109999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>25.9</v>
+        <v>11.7</v>
       </c>
       <c r="C6">
-        <v>2.012</v>
+        <v>14.2</v>
       </c>
       <c r="D6">
-        <v>29.872</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="E6">
-        <v>11.175000000000001</v>
+        <v>1.81</v>
       </c>
       <c r="F6">
-        <v>11.501000000000001</v>
+        <v>12.858000000000001</v>
       </c>
       <c r="G6">
-        <v>3.4450000000000003</v>
+        <v>17.013999999999999</v>
       </c>
       <c r="H6">
-        <v>4.7889999999999997</v>
+        <v>2.387</v>
       </c>
       <c r="I6">
-        <v>11.177</v>
+        <v>8.7880000000000003</v>
       </c>
       <c r="J6">
-        <v>21.161999999999999</v>
+        <v>2.4630000000000001</v>
       </c>
       <c r="K6">
-        <v>15.030999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9.0380000000000003</v>
+      </c>
+      <c r="L6">
+        <v>1.673</v>
+      </c>
+      <c r="M6">
+        <v>1.772</v>
+      </c>
+      <c r="N6">
+        <v>1.44</v>
+      </c>
+      <c r="O6">
+        <v>3.3490000000000002</v>
+      </c>
+      <c r="P6">
+        <v>5.9829999999999997</v>
+      </c>
+      <c r="Q6">
+        <v>5.194</v>
+      </c>
+      <c r="R6">
+        <v>1.6439999999999999</v>
+      </c>
+      <c r="S6">
+        <v>19.518000000000001</v>
+      </c>
+      <c r="T6">
+        <v>5.2869999999999999</v>
+      </c>
+      <c r="U6">
+        <v>9.7439999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.995</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="C7">
-        <v>0.995</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="D7">
-        <v>4.0629999999999997</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="E7">
-        <v>2.96</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="F7">
-        <v>15.744</v>
+        <v>3.125</v>
       </c>
       <c r="G7">
-        <v>8.5210000000000008</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="H7">
-        <v>5.2050000000000001</v>
+        <v>1.1850000000000001</v>
       </c>
       <c r="I7">
-        <v>0.995</v>
+        <v>1.7749999999999999</v>
       </c>
       <c r="J7">
-        <v>1.5529999999999999</v>
+        <v>14.372999999999999</v>
       </c>
       <c r="K7">
-        <v>4.3549999999999995</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.371</v>
+      </c>
+      <c r="L7">
+        <v>3.2210000000000001</v>
+      </c>
+      <c r="M7">
+        <v>5.3</v>
+      </c>
+      <c r="N7">
+        <v>2.81</v>
+      </c>
+      <c r="O7">
+        <v>2.395</v>
+      </c>
+      <c r="P7">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="Q7">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="R7">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="S7">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="T7">
+        <v>2.5459999999999998</v>
+      </c>
+      <c r="U7">
+        <v>1.8089999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>6.4379999999999997</v>
+        <v>4.1529999999999996</v>
       </c>
       <c r="C8">
-        <v>1.5489999999999999</v>
+        <v>2.2850000000000001</v>
       </c>
       <c r="D8">
-        <v>2.3689999999999998</v>
+        <v>0.61099999999999999</v>
       </c>
       <c r="E8">
-        <v>1.6389999999999998</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="F8">
-        <v>2.76</v>
+        <v>1.0720000000000001</v>
       </c>
       <c r="G8">
-        <v>1.306</v>
+        <v>1.2969999999999999</v>
       </c>
       <c r="H8">
-        <v>1.758</v>
+        <v>0.70099999999999996</v>
       </c>
       <c r="I8">
-        <v>2.5990000000000002</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="J8">
-        <v>2.4550000000000001</v>
+        <v>1.8220000000000001</v>
       </c>
       <c r="K8">
-        <v>4.3220000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="L8">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="M8">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="N8">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="O8">
+        <v>1.7010000000000001</v>
+      </c>
+      <c r="P8">
+        <v>1.661</v>
+      </c>
+      <c r="Q8">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="R8">
+        <v>1.5169999999999999</v>
+      </c>
+      <c r="S8">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="T8">
+        <v>3.3839999999999999</v>
+      </c>
+      <c r="U8">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1.597</v>
+        <v>0.65900000000000003</v>
       </c>
       <c r="C9">
-        <v>1.536</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="D9">
-        <v>1.8079999999999998</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="E9">
-        <v>3.3540000000000001</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="F9">
-        <v>1.393</v>
+        <v>0.87</v>
       </c>
       <c r="G9">
-        <v>7.2930000000000001</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="H9">
-        <v>2.214</v>
+        <v>2.4159999999999999</v>
       </c>
       <c r="I9">
-        <v>17.420000000000002</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="J9">
-        <v>5.0220000000000002</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="K9">
-        <v>6.1609999999999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="L9">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="M9">
+        <v>7.2359999999999998</v>
+      </c>
+      <c r="N9">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="O9">
+        <v>2.157</v>
+      </c>
+      <c r="P9">
+        <v>13.305</v>
+      </c>
+      <c r="Q9">
+        <v>4.1150000000000002</v>
+      </c>
+      <c r="R9">
+        <v>3.8010000000000002</v>
+      </c>
+      <c r="S9">
+        <v>1.2210000000000001</v>
+      </c>
+      <c r="T9">
+        <v>3.484</v>
+      </c>
+      <c r="U9">
+        <v>2.677</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>3.6369999999999996</v>
+        <v>2.6989999999999998</v>
       </c>
       <c r="C10">
-        <v>1.7609999999999999</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="D10">
-        <v>0.995</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="E10">
-        <v>7.577</v>
+        <v>1.704</v>
       </c>
       <c r="F10">
-        <v>1.8580000000000001</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="G10">
-        <v>8.9239999999999995</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="H10">
-        <v>0.995</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="I10">
-        <v>0.995</v>
+        <v>7.52</v>
       </c>
       <c r="J10">
-        <v>1.8169999999999999</v>
+        <v>0.92</v>
       </c>
       <c r="K10">
-        <v>2.113</v>
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="L10">
+        <v>1.3240000000000001</v>
+      </c>
+      <c r="M10">
+        <v>7.6</v>
+      </c>
+      <c r="N10">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="O10">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="P10">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="Q10">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="R10">
+        <v>0.879</v>
+      </c>
+      <c r="S10">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="T10">
+        <v>1.175</v>
+      </c>
+      <c r="U10">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13">
+        <v>0.85599999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <f>B2*$D$13 + C2</f>
+        <v>3.9959120000000001</v>
+      </c>
+      <c r="C21">
+        <f>D2*$D$13 + E2</f>
+        <v>10.940488</v>
+      </c>
+      <c r="D21">
+        <f>F2*$D$13 + G2</f>
+        <v>3.004912</v>
+      </c>
+      <c r="E21">
+        <f>H2*$D$13 + I2</f>
+        <v>0.9919119999999999</v>
+      </c>
+      <c r="F21">
+        <f>J2*$D$13 + K2</f>
+        <v>6.0076959999999993</v>
+      </c>
+      <c r="G21">
+        <f>L2*$D$13 + M2</f>
+        <v>0.79091200000000006</v>
+      </c>
+      <c r="H21">
+        <f>N2*$D$13 + O2</f>
+        <v>4.9704239999999995</v>
+      </c>
+      <c r="I21">
+        <f>P2*$D$13 + Q2</f>
+        <v>0.79091200000000006</v>
+      </c>
+      <c r="J21">
+        <f>R2*$D$13 + S2</f>
+        <v>4.1629360000000002</v>
+      </c>
+      <c r="K21">
+        <f>T2*$D$13 + U2</f>
+        <v>12.784552</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <f>B3*$D$13 + C3</f>
+        <v>6.855232</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:C29" si="0">D3*$D$13 + E3</f>
+        <v>9.6488960000000006</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22:E29" si="1">H3*$D$13 + I3</f>
+        <v>12.886912000000001</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ref="F22:F29" si="2">J3*$D$13 + K3</f>
+        <v>6.4102320000000006</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ref="G22:G29" si="3">L3*$D$13 + M3</f>
+        <v>21.202088</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ref="H22:H29" si="4">N3*$D$13 + O3</f>
+        <v>11.283896</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ref="I22:I29" si="5">P3*$D$13 + Q3</f>
+        <v>50.448912</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ref="J22:J29" si="6">R3*$D$13 + S3</f>
+        <v>16.773232</v>
+      </c>
+      <c r="K22">
+        <f t="shared" ref="K22:K29" si="7">T3*$D$13 + U3</f>
+        <v>11.950175999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <f>B4*$D$13 + C4</f>
+        <v>32.389944</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>9.6306079999999987</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D22:D29" si="8">F4*$D$13 + G4</f>
+        <v>63.242655999999997</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>20.55968</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>13.677327999999999</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>12.447824000000001</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="4"/>
+        <v>25.116432</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="5"/>
+        <v>14.799455999999999</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="6"/>
+        <v>52.232352000000006</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="7"/>
+        <v>28.251456000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <f>B5*$D$13 + C5</f>
+        <v>20.620664000000001</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>10.355560000000001</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="8"/>
+        <v>3.410272</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>47.986695999999995</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>13.750872000000001</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>8.3715679999999999</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="4"/>
+        <v>12.168455999999999</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="5"/>
+        <v>5.9644960000000005</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="6"/>
+        <v>9.902864000000001</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="7"/>
+        <v>22.926471999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <f>B6*$D$13 + C6</f>
+        <v>24.215199999999996</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>1.982912</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="8"/>
+        <v>28.020448000000002</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>10.831272</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>11.146328</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>3.204088</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="4"/>
+        <v>4.5816400000000002</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="5"/>
+        <v>10.315448</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="6"/>
+        <v>20.925264000000002</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="7"/>
+        <v>14.269672</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <f>B7*$D$13 + C7</f>
+        <v>0.98679199999999989</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>0.98679199999999989</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="8"/>
+        <v>3.6129999999999995</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>2.7893599999999998</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>13.674287999999999</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>8.0571760000000001</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="4"/>
+        <v>4.8003599999999995</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="5"/>
+        <v>0.98679199999999989</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="6"/>
+        <v>1.46444</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="7"/>
+        <v>3.9883759999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <f>B8*$D$13 + C8</f>
+        <v>5.8399679999999998</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>1.4610159999999999</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="8"/>
+        <v>2.2146319999999999</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>1.5380559999999999</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>2.4976320000000003</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>1.2530079999999999</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="4"/>
+        <v>1.749792</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="5"/>
+        <v>2.3598159999999999</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="6"/>
+        <v>2.2365519999999997</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="7"/>
+        <v>3.8347039999999994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <f>B9*$D$13 + C9</f>
+        <v>1.5021040000000001</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>1.4498880000000001</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="8"/>
+        <v>1.6827199999999998</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>3.0060959999999994</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>1.32748</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>7.2847919999999995</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="4"/>
+        <v>2.2057920000000002</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="5"/>
+        <v>15.50408</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="6"/>
+        <v>4.4746559999999995</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="7"/>
+        <v>5.6593040000000006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <f>B10*$D$13 + C10</f>
+        <v>3.2483439999999995</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>1.7527919999999999</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="8"/>
+        <v>0.98679199999999989</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>7.5687919999999993</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>1.7255199999999999</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>8.7333439999999989</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="4"/>
+        <v>0.98679199999999989</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="5"/>
+        <v>0.98679199999999989</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="6"/>
+        <v>1.6904239999999999</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="7"/>
+        <v>1.9438</v>
       </c>
     </row>
   </sheetData>
@@ -820,17 +1625,359 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>21</v>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3.9959120000000001</v>
+      </c>
+      <c r="C2">
+        <v>10.940488</v>
+      </c>
+      <c r="D2">
+        <v>3.004912</v>
+      </c>
+      <c r="E2">
+        <v>0.9919119999999999</v>
+      </c>
+      <c r="F2">
+        <v>6.0076959999999993</v>
+      </c>
+      <c r="G2">
+        <v>0.79091200000000006</v>
+      </c>
+      <c r="H2">
+        <v>4.9704239999999995</v>
+      </c>
+      <c r="I2">
+        <v>0.79091200000000006</v>
+      </c>
+      <c r="J2">
+        <v>4.1629360000000002</v>
+      </c>
+      <c r="K2">
+        <v>12.784552</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>6.855232</v>
+      </c>
+      <c r="C3">
+        <v>9.6488960000000006</v>
+      </c>
+      <c r="E3">
+        <v>12.886912000000001</v>
+      </c>
+      <c r="F3">
+        <v>6.4102320000000006</v>
+      </c>
+      <c r="G3">
+        <v>21.202088</v>
+      </c>
+      <c r="H3">
+        <v>11.283896</v>
+      </c>
+      <c r="I3">
+        <v>50.448912</v>
+      </c>
+      <c r="J3">
+        <v>16.773232</v>
+      </c>
+      <c r="K3">
+        <v>11.950175999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>32.389944</v>
+      </c>
+      <c r="C4">
+        <v>9.6306079999999987</v>
+      </c>
+      <c r="D4">
+        <v>63.242655999999997</v>
+      </c>
+      <c r="E4">
+        <v>20.55968</v>
+      </c>
+      <c r="F4">
+        <v>13.677327999999999</v>
+      </c>
+      <c r="G4">
+        <v>12.447824000000001</v>
+      </c>
+      <c r="H4">
+        <v>25.116432</v>
+      </c>
+      <c r="I4">
+        <v>14.799455999999999</v>
+      </c>
+      <c r="J4">
+        <v>52.232352000000006</v>
+      </c>
+      <c r="K4">
+        <v>28.251456000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>20.620664000000001</v>
+      </c>
+      <c r="C5">
+        <v>10.355560000000001</v>
+      </c>
+      <c r="D5">
+        <v>3.410272</v>
+      </c>
+      <c r="E5">
+        <v>47.986695999999995</v>
+      </c>
+      <c r="F5">
+        <v>13.750872000000001</v>
+      </c>
+      <c r="G5">
+        <v>8.3715679999999999</v>
+      </c>
+      <c r="H5">
+        <v>12.168455999999999</v>
+      </c>
+      <c r="I5">
+        <v>5.9644960000000005</v>
+      </c>
+      <c r="J5">
+        <v>9.902864000000001</v>
+      </c>
+      <c r="K5">
+        <v>22.926471999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>24.215199999999996</v>
+      </c>
+      <c r="C6">
+        <v>1.982912</v>
+      </c>
+      <c r="D6">
+        <v>28.020448000000002</v>
+      </c>
+      <c r="E6">
+        <v>10.831272</v>
+      </c>
+      <c r="F6">
+        <v>11.146328</v>
+      </c>
+      <c r="G6">
+        <v>3.204088</v>
+      </c>
+      <c r="H6">
+        <v>4.5816400000000002</v>
+      </c>
+      <c r="I6">
+        <v>10.315448</v>
+      </c>
+      <c r="J6">
+        <v>20.925264000000002</v>
+      </c>
+      <c r="K6">
+        <v>14.269672</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.98679199999999989</v>
+      </c>
+      <c r="C7">
+        <v>0.98679199999999989</v>
+      </c>
+      <c r="D7">
+        <v>3.6129999999999995</v>
+      </c>
+      <c r="E7">
+        <v>2.7893599999999998</v>
+      </c>
+      <c r="F7">
+        <v>13.674287999999999</v>
+      </c>
+      <c r="G7">
+        <v>8.0571760000000001</v>
+      </c>
+      <c r="H7">
+        <v>4.8003599999999995</v>
+      </c>
+      <c r="I7">
+        <v>0.98679199999999989</v>
+      </c>
+      <c r="J7">
+        <v>1.46444</v>
+      </c>
+      <c r="K7">
+        <v>3.9883759999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>5.8399679999999998</v>
+      </c>
+      <c r="C8">
+        <v>1.4610159999999999</v>
+      </c>
+      <c r="D8">
+        <v>2.2146319999999999</v>
+      </c>
+      <c r="E8">
+        <v>1.5380559999999999</v>
+      </c>
+      <c r="F8">
+        <v>2.4976320000000003</v>
+      </c>
+      <c r="G8">
+        <v>1.2530079999999999</v>
+      </c>
+      <c r="H8">
+        <v>1.749792</v>
+      </c>
+      <c r="I8">
+        <v>2.3598159999999999</v>
+      </c>
+      <c r="J8">
+        <v>2.2365519999999997</v>
+      </c>
+      <c r="K8">
+        <v>3.8347039999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1.5021040000000001</v>
+      </c>
+      <c r="C9">
+        <v>1.4498880000000001</v>
+      </c>
+      <c r="D9">
+        <v>1.6827199999999998</v>
+      </c>
+      <c r="E9">
+        <v>3.0060959999999994</v>
+      </c>
+      <c r="F9">
+        <v>1.32748</v>
+      </c>
+      <c r="G9">
+        <v>7.2847919999999995</v>
+      </c>
+      <c r="H9">
+        <v>2.2057920000000002</v>
+      </c>
+      <c r="I9">
+        <v>15.50408</v>
+      </c>
+      <c r="J9">
+        <v>4.4746559999999995</v>
+      </c>
+      <c r="K9">
+        <v>5.6593040000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3.2483439999999995</v>
+      </c>
+      <c r="C10">
+        <v>1.7527919999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.98679199999999989</v>
+      </c>
+      <c r="E10">
+        <v>7.5687919999999993</v>
+      </c>
+      <c r="F10">
+        <v>1.7255199999999999</v>
+      </c>
+      <c r="G10">
+        <v>8.7333439999999989</v>
+      </c>
+      <c r="H10">
+        <v>0.98679199999999989</v>
+      </c>
+      <c r="I10">
+        <v>0.98679199999999989</v>
+      </c>
+      <c r="J10">
+        <v>1.6904239999999999</v>
+      </c>
+      <c r="K10">
+        <v>1.9438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data on neonic means and peaks for each site
</commit_message>
<xml_diff>
--- a/data/raw/field_neonic_exposure.xlsx
+++ b/data/raw/field_neonic_exposure.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_files\minucci_vp_mcmc\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="raw neonic pollen" sheetId="1" r:id="rId1"/>
     <sheet name="raw neonic clo equivalents" sheetId="2" r:id="rId2"/>
+    <sheet name="clo equivalent means and peaks" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -154,6 +155,15 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Peak</t>
+  </si>
+  <si>
+    <t>Site</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1231,7 @@
         <v>1</v>
       </c>
       <c r="B21">
-        <f>B2*$D$13 + C2</f>
+        <f t="shared" ref="B21:B29" si="0">B2*$D$13 + C2</f>
         <v>3.9959120000000001</v>
       </c>
       <c r="C21">
@@ -1266,39 +1276,39 @@
         <v>2</v>
       </c>
       <c r="B22">
-        <f>B3*$D$13 + C3</f>
+        <f t="shared" si="0"/>
         <v>6.855232</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:C29" si="0">D3*$D$13 + E3</f>
+        <f t="shared" ref="C22:C29" si="1">D3*$D$13 + E3</f>
         <v>9.6488960000000006</v>
       </c>
       <c r="E22">
-        <f t="shared" ref="E22:E29" si="1">H3*$D$13 + I3</f>
+        <f t="shared" ref="E22:E29" si="2">H3*$D$13 + I3</f>
         <v>12.886912000000001</v>
       </c>
       <c r="F22">
-        <f t="shared" ref="F22:F29" si="2">J3*$D$13 + K3</f>
+        <f t="shared" ref="F22:F29" si="3">J3*$D$13 + K3</f>
         <v>6.4102320000000006</v>
       </c>
       <c r="G22">
-        <f t="shared" ref="G22:G29" si="3">L3*$D$13 + M3</f>
+        <f t="shared" ref="G22:G29" si="4">L3*$D$13 + M3</f>
         <v>21.202088</v>
       </c>
       <c r="H22">
-        <f t="shared" ref="H22:H29" si="4">N3*$D$13 + O3</f>
+        <f t="shared" ref="H22:H29" si="5">N3*$D$13 + O3</f>
         <v>11.283896</v>
       </c>
       <c r="I22">
-        <f t="shared" ref="I22:I29" si="5">P3*$D$13 + Q3</f>
+        <f t="shared" ref="I22:I29" si="6">P3*$D$13 + Q3</f>
         <v>50.448912</v>
       </c>
       <c r="J22">
-        <f t="shared" ref="J22:J29" si="6">R3*$D$13 + S3</f>
+        <f t="shared" ref="J22:J29" si="7">R3*$D$13 + S3</f>
         <v>16.773232</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22:K29" si="7">T3*$D$13 + U3</f>
+        <f t="shared" ref="K22:K29" si="8">T3*$D$13 + U3</f>
         <v>11.950175999999999</v>
       </c>
     </row>
@@ -1307,43 +1317,43 @@
         <v>3</v>
       </c>
       <c r="B23">
-        <f>B4*$D$13 + C4</f>
+        <f t="shared" si="0"/>
         <v>32.389944</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.6306079999999987</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D22:D29" si="8">F4*$D$13 + G4</f>
+        <f t="shared" ref="D23:D29" si="9">F4*$D$13 + G4</f>
         <v>63.242655999999997</v>
       </c>
       <c r="E23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20.55968</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.677327999999999</v>
       </c>
       <c r="G23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12.447824000000001</v>
       </c>
       <c r="H23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>25.116432</v>
       </c>
       <c r="I23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14.799455999999999</v>
       </c>
       <c r="J23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>52.232352000000006</v>
       </c>
       <c r="K23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28.251456000000001</v>
       </c>
     </row>
@@ -1352,43 +1362,43 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <f>B5*$D$13 + C5</f>
+        <f t="shared" si="0"/>
         <v>20.620664000000001</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.355560000000001</v>
       </c>
       <c r="D24">
+        <f t="shared" si="9"/>
+        <v>3.410272</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>47.986695999999995</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>13.750872000000001</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="4"/>
+        <v>8.3715679999999999</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="5"/>
+        <v>12.168455999999999</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="6"/>
+        <v>5.9644960000000005</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="7"/>
+        <v>9.902864000000001</v>
+      </c>
+      <c r="K24">
         <f t="shared" si="8"/>
-        <v>3.410272</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="1"/>
-        <v>47.986695999999995</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="2"/>
-        <v>13.750872000000001</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="3"/>
-        <v>8.3715679999999999</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="4"/>
-        <v>12.168455999999999</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="5"/>
-        <v>5.9644960000000005</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="6"/>
-        <v>9.902864000000001</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="7"/>
         <v>22.926471999999997</v>
       </c>
     </row>
@@ -1397,43 +1407,43 @@
         <v>5</v>
       </c>
       <c r="B25">
-        <f>B6*$D$13 + C6</f>
+        <f t="shared" si="0"/>
         <v>24.215199999999996</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.982912</v>
       </c>
       <c r="D25">
+        <f t="shared" si="9"/>
+        <v>28.020448000000002</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>10.831272</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="3"/>
+        <v>11.146328</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="4"/>
+        <v>3.204088</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="5"/>
+        <v>4.5816400000000002</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="6"/>
+        <v>10.315448</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="7"/>
+        <v>20.925264000000002</v>
+      </c>
+      <c r="K25">
         <f t="shared" si="8"/>
-        <v>28.020448000000002</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="1"/>
-        <v>10.831272</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="2"/>
-        <v>11.146328</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="3"/>
-        <v>3.204088</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="4"/>
-        <v>4.5816400000000002</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="5"/>
-        <v>10.315448</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="6"/>
-        <v>20.925264000000002</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="7"/>
         <v>14.269672</v>
       </c>
     </row>
@@ -1442,43 +1452,43 @@
         <v>6</v>
       </c>
       <c r="B26">
-        <f>B7*$D$13 + C7</f>
-        <v>0.98679199999999989</v>
-      </c>
-      <c r="C26">
         <f t="shared" si="0"/>
         <v>0.98679199999999989</v>
       </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>0.98679199999999989</v>
+      </c>
       <c r="D26">
+        <f t="shared" si="9"/>
+        <v>3.6129999999999995</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>2.7893599999999998</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="3"/>
+        <v>13.674287999999999</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>8.0571760000000001</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="5"/>
+        <v>4.8003599999999995</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="6"/>
+        <v>0.98679199999999989</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="7"/>
+        <v>1.46444</v>
+      </c>
+      <c r="K26">
         <f t="shared" si="8"/>
-        <v>3.6129999999999995</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="1"/>
-        <v>2.7893599999999998</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="2"/>
-        <v>13.674287999999999</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="3"/>
-        <v>8.0571760000000001</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="4"/>
-        <v>4.8003599999999995</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="5"/>
-        <v>0.98679199999999989</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="6"/>
-        <v>1.46444</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="7"/>
         <v>3.9883759999999997</v>
       </c>
     </row>
@@ -1487,43 +1497,43 @@
         <v>7</v>
       </c>
       <c r="B27">
-        <f>B8*$D$13 + C8</f>
+        <f t="shared" si="0"/>
         <v>5.8399679999999998</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4610159999999999</v>
       </c>
       <c r="D27">
+        <f t="shared" si="9"/>
+        <v>2.2146319999999999</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>1.5380559999999999</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="3"/>
+        <v>2.4976320000000003</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="4"/>
+        <v>1.2530079999999999</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="5"/>
+        <v>1.749792</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="6"/>
+        <v>2.3598159999999999</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="7"/>
+        <v>2.2365519999999997</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="8"/>
-        <v>2.2146319999999999</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="1"/>
-        <v>1.5380559999999999</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="2"/>
-        <v>2.4976320000000003</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="3"/>
-        <v>1.2530079999999999</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="4"/>
-        <v>1.749792</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="5"/>
-        <v>2.3598159999999999</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="6"/>
-        <v>2.2365519999999997</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="7"/>
         <v>3.8347039999999994</v>
       </c>
     </row>
@@ -1532,43 +1542,43 @@
         <v>8</v>
       </c>
       <c r="B28">
-        <f>B9*$D$13 + C9</f>
+        <f t="shared" si="0"/>
         <v>1.5021040000000001</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4498880000000001</v>
       </c>
       <c r="D28">
+        <f t="shared" si="9"/>
+        <v>1.6827199999999998</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>3.0060959999999994</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="3"/>
+        <v>1.32748</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="4"/>
+        <v>7.2847919999999995</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="5"/>
+        <v>2.2057920000000002</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="6"/>
+        <v>15.50408</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="7"/>
+        <v>4.4746559999999995</v>
+      </c>
+      <c r="K28">
         <f t="shared" si="8"/>
-        <v>1.6827199999999998</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="1"/>
-        <v>3.0060959999999994</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="2"/>
-        <v>1.32748</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="3"/>
-        <v>7.2847919999999995</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="4"/>
-        <v>2.2057920000000002</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="5"/>
-        <v>15.50408</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="6"/>
-        <v>4.4746559999999995</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="7"/>
         <v>5.6593040000000006</v>
       </c>
     </row>
@@ -1577,43 +1587,43 @@
         <v>9</v>
       </c>
       <c r="B29">
-        <f>B10*$D$13 + C10</f>
+        <f t="shared" si="0"/>
         <v>3.2483439999999995</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7527919999999999</v>
       </c>
       <c r="D29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.98679199999999989</v>
       </c>
       <c r="E29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.5687919999999993</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.7255199999999999</v>
       </c>
       <c r="G29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.7333439999999989</v>
       </c>
       <c r="H29">
-        <f t="shared" si="4"/>
-        <v>0.98679199999999989</v>
-      </c>
-      <c r="I29">
         <f t="shared" si="5"/>
         <v>0.98679199999999989</v>
       </c>
+      <c r="I29">
+        <f t="shared" si="6"/>
+        <v>0.98679199999999989</v>
+      </c>
       <c r="J29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6904239999999999</v>
       </c>
       <c r="K29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.9438</v>
       </c>
     </row>
@@ -1625,10 +1635,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1980,6 +1990,232 @@
         <v>1.9438</v>
       </c>
     </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12">
+        <f>AVERAGE(B2:B10)</f>
+        <v>11.072684444444443</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:K12" si="0">AVERAGE(C2:C10)</f>
+        <v>5.3565502222222223</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>13.271929</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>12.017641777777776</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>7.8019306666666672</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>7.9272000000000009</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>7.5403982222222208</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>11.350744888888887</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>12.651413333333331</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>11.734279111111112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13">
+        <f>MAX(B2:B10)</f>
+        <v>32.389944</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:K13" si="1">MAX(C2:C10)</f>
+        <v>10.940488</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>63.242655999999997</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>47.986695999999995</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>13.750872000000001</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>21.202088</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>25.116432</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>50.448912</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>52.232352000000006</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>28.251456000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>11.072684444444443</v>
+      </c>
+      <c r="C2">
+        <v>32.389944</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>5.3565502222222223</v>
+      </c>
+      <c r="C3">
+        <v>10.940488</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>13.271929</v>
+      </c>
+      <c r="C4">
+        <v>63.242655999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>12.017641777777776</v>
+      </c>
+      <c r="C5">
+        <v>47.986695999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>7.8019306666666672</v>
+      </c>
+      <c r="C6">
+        <v>13.750872000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>7.9272000000000009</v>
+      </c>
+      <c r="C7">
+        <v>21.202088</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8">
+        <v>7.5403982222222208</v>
+      </c>
+      <c r="C8">
+        <v>25.116432</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>11.350744888888887</v>
+      </c>
+      <c r="C9">
+        <v>50.448912</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>12.651413333333331</v>
+      </c>
+      <c r="C10">
+        <v>52.232352000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>11.734279111111112</v>
+      </c>
+      <c r="C11">
+        <v>28.251456000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>